<commit_message>
Updating to support publishing to prod.
</commit_message>
<xml_diff>
--- a/docs/Project Details.xlsx
+++ b/docs/Project Details.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="17970" windowHeight="24915"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="17970" windowHeight="24915" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
-    <sheet name="Poker Hand Rankings" sheetId="2" r:id="rId2"/>
-    <sheet name="Odds" sheetId="4" r:id="rId3"/>
+    <sheet name="Winning Hands JSON" sheetId="5" r:id="rId2"/>
+    <sheet name="Poker Hand Rankings" sheetId="2" r:id="rId3"/>
+    <sheet name="Odds" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="140">
   <si>
     <t>Investigate ECMAScript instead of Lodash</t>
   </si>
@@ -338,6 +339,114 @@
   </si>
   <si>
     <t>Create unit tests  for sorter, evaluator, etc.</t>
+  </si>
+  <si>
+    <t>isSequence</t>
+  </si>
+  <si>
+    <t>isSameSuit</t>
+  </si>
+  <si>
+    <t>sameTwoRank</t>
+  </si>
+  <si>
+    <t>sameThreeRank</t>
+  </si>
+  <si>
+    <t>sameFourRank</t>
+  </si>
+  <si>
+    <t>tieBreaker</t>
+  </si>
+  <si>
+    <t>Four of a Kind</t>
+  </si>
+  <si>
+    <t>!= Ace</t>
+  </si>
+  <si>
+    <t>HighPair</t>
+  </si>
+  <si>
+    <t>Highest "SameThreeRank"</t>
+  </si>
+  <si>
+    <t>Highest 5th card</t>
+  </si>
+  <si>
+    <t>requiredCard</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>name: "Royal Flush",</t>
+  </si>
+  <si>
+    <t>rank: 1,</t>
+  </si>
+  <si>
+    <t>formula: {</t>
+  </si>
+  <si>
+    <t>isSequence: true,</t>
+  </si>
+  <si>
+    <t>isSameSuit: true,</t>
+  </si>
+  <si>
+    <t>sameTwoRank: 0,</t>
+  </si>
+  <si>
+    <t>sameThreeRank: 0,</t>
+  </si>
+  <si>
+    <t>sameFourRank: 0,</t>
+  </si>
+  <si>
+    <t>requiredCard: "Ace",</t>
+  </si>
+  <si>
+    <t>tieBreaker: ""</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>[{</t>
+  </si>
+  <si>
+    <t>}, …</t>
+  </si>
+  <si>
+    <t>pokerHands.json</t>
+  </si>
+  <si>
+    <t>formulas using commands</t>
+  </si>
+  <si>
+    <t>formulas: [{</t>
+  </si>
+  <si>
+    <t>name: "isSequence",</t>
+  </si>
+  <si>
+    <t>value: true</t>
+  </si>
+  <si>
+    <t>}, {</t>
+  </si>
+  <si>
+    <t>name: "isSameSuit",</t>
+  </si>
+  <si>
+    <t>name: "requiredCard",</t>
+  </si>
+  <si>
+    <t>value: "Ace"</t>
+  </si>
+  <si>
+    <t>}]</t>
   </si>
 </sst>
 </file>
@@ -419,7 +528,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -488,12 +597,93 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -514,6 +704,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -523,6 +723,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -530,15 +739,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -550,16 +750,36 @@
     <xf numFmtId="9" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4118,7 +4338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -4299,7 +4519,7 @@
       <c r="B17" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="12" t="s">
         <v>93</v>
       </c>
     </row>
@@ -4354,7 +4574,7 @@
       <c r="B25" t="s">
         <v>103</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="12" t="s">
         <v>95</v>
       </c>
     </row>
@@ -4365,7 +4585,7 @@
       <c r="B26" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="12" t="s">
         <v>95</v>
       </c>
     </row>
@@ -4483,6 +4703,421 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:K40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" style="31" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" s="36" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="35"/>
+      <c r="B2" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="K3" s="34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="J4" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="K4" s="29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="30">
+        <v>0</v>
+      </c>
+      <c r="C5" s="29">
+        <v>0</v>
+      </c>
+      <c r="D5" s="29">
+        <v>0</v>
+      </c>
+      <c r="E5" s="37">
+        <v>1</v>
+      </c>
+      <c r="F5" s="29">
+        <v>0</v>
+      </c>
+      <c r="G5" s="29">
+        <v>0</v>
+      </c>
+      <c r="H5" s="29">
+        <v>0</v>
+      </c>
+      <c r="I5" s="37">
+        <v>2</v>
+      </c>
+      <c r="J5" s="37">
+        <v>1</v>
+      </c>
+      <c r="K5" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="30">
+        <v>0</v>
+      </c>
+      <c r="C6" s="29">
+        <v>0</v>
+      </c>
+      <c r="D6" s="29">
+        <v>0</v>
+      </c>
+      <c r="E6" s="37">
+        <v>1</v>
+      </c>
+      <c r="F6" s="29">
+        <v>0</v>
+      </c>
+      <c r="G6" s="29">
+        <v>0</v>
+      </c>
+      <c r="H6" s="37">
+        <v>1</v>
+      </c>
+      <c r="I6" s="29">
+        <v>0</v>
+      </c>
+      <c r="J6" s="29">
+        <v>0</v>
+      </c>
+      <c r="K6" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="30">
+        <v>0</v>
+      </c>
+      <c r="C7" s="29">
+        <v>0</v>
+      </c>
+      <c r="D7" s="37">
+        <v>4</v>
+      </c>
+      <c r="E7" s="29">
+        <v>0</v>
+      </c>
+      <c r="F7" s="29">
+        <v>0</v>
+      </c>
+      <c r="G7" s="29">
+        <v>0</v>
+      </c>
+      <c r="H7" s="29">
+        <v>0</v>
+      </c>
+      <c r="I7" s="29">
+        <v>0</v>
+      </c>
+      <c r="J7" s="29">
+        <v>0</v>
+      </c>
+      <c r="K7" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="39" t="str">
+        <f>TEXT("==Ace","")</f>
+        <v>==Ace</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+    </row>
+    <row r="9" spans="1:11" s="28" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="41"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="K9" s="42"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E45"/>
   <sheetViews>
@@ -4855,7 +5490,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F73"/>
   <sheetViews>
@@ -4903,687 +5538,735 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="13">
         <v>1</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="13">
         <v>4</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="19">
         <v>1.5400000000000001E-6</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="19">
         <v>1.5400000000000001E-6</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="25"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="25"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="25"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="25"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="25"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="26"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="15"/>
     </row>
     <row r="11" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="13">
         <v>9</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="13">
         <v>36</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="19">
         <v>1.3900000000000001E-5</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="19">
         <v>1.5E-5</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="13" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="25"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="25"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="25"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="25"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="25"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="26"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="13">
         <v>156</v>
       </c>
-      <c r="C18" s="24">
+      <c r="C18" s="13">
         <v>624</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="19">
         <v>2.4000000000000001E-4</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="19">
         <v>2.5599999999999999E-4</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F18" s="13" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="25"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="14"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="25"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="14"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="25"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="25"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="25"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="26"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="15"/>
     </row>
     <row r="25" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="24">
+      <c r="B25" s="13">
         <v>156</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="22">
         <v>3744</v>
       </c>
-      <c r="D25" s="18">
+      <c r="D25" s="19">
         <v>1.441E-3</v>
       </c>
-      <c r="E25" s="18">
+      <c r="E25" s="19">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="F25" s="24" t="s">
+      <c r="F25" s="13" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="25"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="25"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="14"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="25"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="14"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="25"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="14"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="25"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="14"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="14"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="26"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="15"/>
     </row>
     <row r="32" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="15">
+      <c r="B32" s="22">
         <v>1277</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="22">
         <v>5108</v>
       </c>
-      <c r="D32" s="18">
+      <c r="D32" s="19">
         <v>1.9650000000000002E-3</v>
       </c>
-      <c r="E32" s="18">
+      <c r="E32" s="19">
         <v>3.6700000000000001E-3</v>
       </c>
-      <c r="F32" s="24" t="s">
+      <c r="F32" s="13" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="25"/>
+      <c r="A33" s="17"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="25"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="25"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="14"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="25"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="14"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="25"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="14"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="14"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="26"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="15"/>
     </row>
     <row r="39" spans="1:6" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B39" s="24">
+      <c r="B39" s="13">
         <v>10</v>
       </c>
-      <c r="C39" s="15">
+      <c r="C39" s="22">
         <v>10200</v>
       </c>
-      <c r="D39" s="18">
+      <c r="D39" s="19">
         <v>3.9249999999999997E-3</v>
       </c>
-      <c r="E39" s="18">
+      <c r="E39" s="19">
         <v>7.6E-3</v>
       </c>
-      <c r="F39" s="24" t="s">
+      <c r="F39" s="13" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="25"/>
+      <c r="A40" s="17"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="14"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="25"/>
+      <c r="A41" s="17"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="14"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="25"/>
+      <c r="A42" s="17"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="14"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="25"/>
+      <c r="A43" s="17"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="14"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="25"/>
+      <c r="A44" s="17"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="14"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="14"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="26"/>
+      <c r="A45" s="18"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="15"/>
     </row>
     <row r="46" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
+      <c r="A46" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B46" s="24">
+      <c r="B46" s="13">
         <v>858</v>
       </c>
-      <c r="C46" s="15">
+      <c r="C46" s="22">
         <v>54912</v>
       </c>
-      <c r="D46" s="18">
+      <c r="D46" s="19">
         <v>2.1128000000000001E-2</v>
       </c>
-      <c r="E46" s="18">
+      <c r="E46" s="19">
         <v>2.87E-2</v>
       </c>
-      <c r="F46" s="24" t="s">
+      <c r="F46" s="13" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="25"/>
+      <c r="A47" s="17"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="14"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="25"/>
+      <c r="A48" s="17"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="14"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="25"/>
+      <c r="A49" s="17"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="14"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="13"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="25"/>
+      <c r="A50" s="17"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="14"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="25"/>
+      <c r="A51" s="17"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="14"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="14"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="26"/>
+      <c r="A52" s="18"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="15"/>
     </row>
     <row r="53" spans="1:6" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="12" t="s">
+      <c r="A53" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B53" s="24">
+      <c r="B53" s="13">
         <v>858</v>
       </c>
-      <c r="C53" s="15">
+      <c r="C53" s="22">
         <v>123552</v>
       </c>
-      <c r="D53" s="18">
+      <c r="D53" s="19">
         <v>4.7538999999999998E-2</v>
       </c>
-      <c r="E53" s="18">
+      <c r="E53" s="19">
         <v>7.6200000000000004E-2</v>
       </c>
-      <c r="F53" s="24" t="s">
+      <c r="F53" s="13" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="25"/>
+      <c r="A54" s="17"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="14"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
-      <c r="B55" s="25"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="25"/>
+      <c r="A55" s="17"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="14"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
-      <c r="B56" s="25"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="25"/>
+      <c r="A56" s="17"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="14"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
-      <c r="B57" s="25"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="25"/>
+      <c r="A57" s="17"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="14"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
-      <c r="B58" s="25"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="25"/>
+      <c r="A58" s="17"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="14"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="14"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="26"/>
+      <c r="A59" s="18"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="15"/>
     </row>
     <row r="60" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="12" t="s">
+      <c r="A60" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B60" s="15">
+      <c r="B60" s="22">
         <v>2860</v>
       </c>
-      <c r="C60" s="15">
+      <c r="C60" s="22">
         <v>1098240</v>
       </c>
-      <c r="D60" s="18">
+      <c r="D60" s="19">
         <v>0.42256899999999997</v>
       </c>
-      <c r="E60" s="18">
+      <c r="E60" s="19">
         <v>0.499</v>
       </c>
-      <c r="F60" s="24" t="s">
+      <c r="F60" s="13" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="19"/>
-      <c r="F61" s="25"/>
+      <c r="A61" s="17"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="14"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="25"/>
+      <c r="A62" s="17"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="14"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
-      <c r="B63" s="16"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="25"/>
+      <c r="A63" s="17"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="14"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
-      <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="25"/>
+      <c r="A64" s="17"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="14"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
-      <c r="B65" s="16"/>
-      <c r="C65" s="16"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="25"/>
+      <c r="A65" s="17"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="14"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="14"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="26"/>
+      <c r="A66" s="18"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="24"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="15"/>
     </row>
     <row r="67" spans="1:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="12" t="s">
+      <c r="A67" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B67" s="15">
+      <c r="B67" s="22">
         <v>1277</v>
       </c>
-      <c r="C67" s="15">
+      <c r="C67" s="22">
         <v>1302540</v>
       </c>
-      <c r="D67" s="18">
+      <c r="D67" s="19">
         <v>0.50117699999999998</v>
       </c>
-      <c r="E67" s="21">
+      <c r="E67" s="25">
         <v>1</v>
       </c>
-      <c r="F67" s="24" t="s">
+      <c r="F67" s="13" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="13"/>
-      <c r="B68" s="16"/>
-      <c r="C68" s="16"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="22"/>
-      <c r="F68" s="25"/>
+      <c r="A68" s="17"/>
+      <c r="B68" s="23"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="14"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
-      <c r="B69" s="16"/>
-      <c r="C69" s="16"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="22"/>
-      <c r="F69" s="25"/>
+      <c r="A69" s="17"/>
+      <c r="B69" s="23"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="14"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
-      <c r="B70" s="16"/>
-      <c r="C70" s="16"/>
-      <c r="D70" s="19"/>
-      <c r="E70" s="22"/>
-      <c r="F70" s="25"/>
+      <c r="A70" s="17"/>
+      <c r="B70" s="23"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="26"/>
+      <c r="F70" s="14"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="13"/>
-      <c r="B71" s="16"/>
-      <c r="C71" s="16"/>
-      <c r="D71" s="19"/>
-      <c r="E71" s="22"/>
-      <c r="F71" s="25"/>
+      <c r="A71" s="17"/>
+      <c r="B71" s="23"/>
+      <c r="C71" s="23"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="14"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="13"/>
-      <c r="B72" s="16"/>
-      <c r="C72" s="16"/>
-      <c r="D72" s="19"/>
-      <c r="E72" s="22"/>
-      <c r="F72" s="25"/>
+      <c r="A72" s="17"/>
+      <c r="B72" s="23"/>
+      <c r="C72" s="23"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="26"/>
+      <c r="F72" s="14"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="14"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="17"/>
-      <c r="D73" s="20"/>
-      <c r="E73" s="23"/>
-      <c r="F73" s="26"/>
+      <c r="A73" s="18"/>
+      <c r="B73" s="24"/>
+      <c r="C73" s="24"/>
+      <c r="D73" s="21"/>
+      <c r="E73" s="27"/>
+      <c r="F73" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="F67:F73"/>
+    <mergeCell ref="A60:A66"/>
+    <mergeCell ref="B60:B66"/>
+    <mergeCell ref="C60:C66"/>
+    <mergeCell ref="D60:D66"/>
+    <mergeCell ref="E60:E66"/>
+    <mergeCell ref="F60:F66"/>
+    <mergeCell ref="A67:A73"/>
+    <mergeCell ref="B67:B73"/>
+    <mergeCell ref="C67:C73"/>
+    <mergeCell ref="D67:D73"/>
+    <mergeCell ref="E67:E73"/>
+    <mergeCell ref="F53:F59"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="C46:C52"/>
+    <mergeCell ref="D46:D52"/>
+    <mergeCell ref="E46:E52"/>
+    <mergeCell ref="F46:F52"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="B53:B59"/>
+    <mergeCell ref="C53:C59"/>
+    <mergeCell ref="D53:D59"/>
+    <mergeCell ref="E53:E59"/>
+    <mergeCell ref="F39:F45"/>
+    <mergeCell ref="A32:A38"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="D32:D38"/>
+    <mergeCell ref="E32:E38"/>
+    <mergeCell ref="F32:F38"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="B39:B45"/>
+    <mergeCell ref="C39:C45"/>
+    <mergeCell ref="D39:D45"/>
+    <mergeCell ref="E39:E45"/>
+    <mergeCell ref="F25:F31"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="C18:C24"/>
+    <mergeCell ref="D18:D24"/>
+    <mergeCell ref="E18:E24"/>
+    <mergeCell ref="F18:F24"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="C25:C31"/>
+    <mergeCell ref="D25:D31"/>
+    <mergeCell ref="E25:E31"/>
     <mergeCell ref="F11:F17"/>
     <mergeCell ref="A4:A10"/>
     <mergeCell ref="B4:B10"/>
@@ -5596,54 +6279,6 @@
     <mergeCell ref="C11:C17"/>
     <mergeCell ref="D11:D17"/>
     <mergeCell ref="E11:E17"/>
-    <mergeCell ref="F25:F31"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="C18:C24"/>
-    <mergeCell ref="D18:D24"/>
-    <mergeCell ref="E18:E24"/>
-    <mergeCell ref="F18:F24"/>
-    <mergeCell ref="A25:A31"/>
-    <mergeCell ref="B25:B31"/>
-    <mergeCell ref="C25:C31"/>
-    <mergeCell ref="D25:D31"/>
-    <mergeCell ref="E25:E31"/>
-    <mergeCell ref="F39:F45"/>
-    <mergeCell ref="A32:A38"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="D32:D38"/>
-    <mergeCell ref="E32:E38"/>
-    <mergeCell ref="F32:F38"/>
-    <mergeCell ref="A39:A45"/>
-    <mergeCell ref="B39:B45"/>
-    <mergeCell ref="C39:C45"/>
-    <mergeCell ref="D39:D45"/>
-    <mergeCell ref="E39:E45"/>
-    <mergeCell ref="F53:F59"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="C46:C52"/>
-    <mergeCell ref="D46:D52"/>
-    <mergeCell ref="E46:E52"/>
-    <mergeCell ref="F46:F52"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="B53:B59"/>
-    <mergeCell ref="C53:C59"/>
-    <mergeCell ref="D53:D59"/>
-    <mergeCell ref="E53:E59"/>
-    <mergeCell ref="F67:F73"/>
-    <mergeCell ref="A60:A66"/>
-    <mergeCell ref="B60:B66"/>
-    <mergeCell ref="C60:C66"/>
-    <mergeCell ref="D60:D66"/>
-    <mergeCell ref="E60:E66"/>
-    <mergeCell ref="F60:F66"/>
-    <mergeCell ref="A67:A73"/>
-    <mergeCell ref="B67:B73"/>
-    <mergeCell ref="C67:C73"/>
-    <mergeCell ref="D67:D73"/>
-    <mergeCell ref="E67:E73"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" location="Straight_flush" tooltip="Hand rankings" display="https://en.wikipedia.org/wiki/Hand_rankings - Straight_flush"/>

</xml_diff>

<commit_message>
Improving model and service architecture.
</commit_message>
<xml_diff>
--- a/docs/Project Details.xlsx
+++ b/docs/Project Details.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="17970" windowHeight="24915" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="17970" windowHeight="24915"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
@@ -705,51 +705,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -779,6 +734,51 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4338,8 +4338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4641,7 +4641,7 @@
         <v>99</v>
       </c>
       <c r="C32" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -4706,265 +4706,265 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" s="36" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35"/>
-      <c r="B2" s="36" t="s">
+    <row r="2" spans="1:11" s="21" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20"/>
+      <c r="B2" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="21" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="I3" s="34" t="s">
+      <c r="I3" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="J3" s="34" t="s">
+      <c r="J3" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="34" t="s">
+      <c r="K3" s="19" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="I4" s="29" t="s">
+      <c r="I4" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="K4" s="29" t="s">
+      <c r="K4" s="14" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="15">
         <v>0</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="14">
         <v>0</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="14">
         <v>0</v>
       </c>
-      <c r="E5" s="37">
+      <c r="E5" s="22">
         <v>1</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="14">
         <v>0</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="14">
         <v>0</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="14">
         <v>0</v>
       </c>
-      <c r="I5" s="37">
+      <c r="I5" s="22">
         <v>2</v>
       </c>
-      <c r="J5" s="37">
+      <c r="J5" s="22">
         <v>1</v>
       </c>
-      <c r="K5" s="29">
+      <c r="K5" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="15">
         <v>0</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="14">
         <v>0</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="14">
         <v>0</v>
       </c>
-      <c r="E6" s="37">
+      <c r="E6" s="22">
         <v>1</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="14">
         <v>0</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="14">
         <v>0</v>
       </c>
-      <c r="H6" s="37">
+      <c r="H6" s="22">
         <v>1</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="14">
         <v>0</v>
       </c>
-      <c r="J6" s="29">
+      <c r="J6" s="14">
         <v>0</v>
       </c>
-      <c r="K6" s="29">
+      <c r="K6" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="15">
         <v>0</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="14">
         <v>0</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="22">
         <v>4</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="14">
         <v>0</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="14">
         <v>0</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="14">
         <v>0</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="14">
         <v>0</v>
       </c>
-      <c r="I7" s="29">
+      <c r="I7" s="14">
         <v>0</v>
       </c>
-      <c r="J7" s="29">
+      <c r="J7" s="14">
         <v>0</v>
       </c>
-      <c r="K7" s="29">
+      <c r="K7" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="B8" s="39" t="str">
+      <c r="B8" s="24" t="str">
         <f>TEXT("==Ace","")</f>
         <v>==Ace</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-    </row>
-    <row r="9" spans="1:11" s="28" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+    </row>
+    <row r="9" spans="1:11" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42" t="s">
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42" t="s">
+      <c r="F9" s="27"/>
+      <c r="G9" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="43" t="s">
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="K9" s="42"/>
+      <c r="K9" s="27"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -5538,687 +5538,735 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="29">
         <v>1</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="29">
         <v>4</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="38">
         <v>1.5400000000000001E-6</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="38">
         <v>1.5400000000000001E-6</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="29" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="14"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="14"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="30"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="14"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="30"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="14"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="30"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="14"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="30"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="15"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="31"/>
     </row>
     <row r="11" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="29">
         <v>9</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="29">
         <v>36</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="38">
         <v>1.3900000000000001E-5</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="38">
         <v>1.5E-5</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="29" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="14"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="30"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="14"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="30"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="14"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="30"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="14"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="30"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="14"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="30"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="15"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="31"/>
     </row>
     <row r="18" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="29">
         <v>156</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="29">
         <v>624</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="38">
         <v>2.4000000000000001E-4</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="38">
         <v>2.5599999999999999E-4</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="29" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="14"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="30"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="14"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="30"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="14"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="30"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="14"/>
+      <c r="A22" s="33"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="30"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="14"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="30"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="18"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="15"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="31"/>
     </row>
     <row r="25" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25" s="29">
         <v>156</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25" s="35">
         <v>3744</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="38">
         <v>1.441E-3</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E25" s="38">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="F25" s="29" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="14"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="30"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="14"/>
+      <c r="A27" s="33"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="30"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="14"/>
+      <c r="A28" s="33"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="30"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="14"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="30"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="14"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="30"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="18"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="15"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="31"/>
     </row>
     <row r="32" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="22">
+      <c r="B32" s="35">
         <v>1277</v>
       </c>
-      <c r="C32" s="22">
+      <c r="C32" s="35">
         <v>5108</v>
       </c>
-      <c r="D32" s="19">
+      <c r="D32" s="38">
         <v>1.9650000000000002E-3</v>
       </c>
-      <c r="E32" s="19">
+      <c r="E32" s="38">
         <v>3.6700000000000001E-3</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="F32" s="29" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="14"/>
+      <c r="A33" s="33"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="30"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="14"/>
+      <c r="A34" s="33"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="30"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="14"/>
+      <c r="A35" s="33"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="30"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="14"/>
+      <c r="A36" s="33"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="30"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="14"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="30"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="18"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="15"/>
+      <c r="A38" s="34"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="31"/>
     </row>
     <row r="39" spans="1:6" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="B39" s="13">
+      <c r="B39" s="29">
         <v>10</v>
       </c>
-      <c r="C39" s="22">
+      <c r="C39" s="35">
         <v>10200</v>
       </c>
-      <c r="D39" s="19">
+      <c r="D39" s="38">
         <v>3.9249999999999997E-3</v>
       </c>
-      <c r="E39" s="19">
+      <c r="E39" s="38">
         <v>7.6E-3</v>
       </c>
-      <c r="F39" s="13" t="s">
+      <c r="F39" s="29" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="14"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="30"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="14"/>
+      <c r="A41" s="33"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="30"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="14"/>
+      <c r="A42" s="33"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="30"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="14"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="30"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="14"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="30"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="18"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="15"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="31"/>
     </row>
     <row r="46" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="16" t="s">
+      <c r="A46" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="B46" s="13">
+      <c r="B46" s="29">
         <v>858</v>
       </c>
-      <c r="C46" s="22">
+      <c r="C46" s="35">
         <v>54912</v>
       </c>
-      <c r="D46" s="19">
+      <c r="D46" s="38">
         <v>2.1128000000000001E-2</v>
       </c>
-      <c r="E46" s="19">
+      <c r="E46" s="38">
         <v>2.87E-2</v>
       </c>
-      <c r="F46" s="13" t="s">
+      <c r="F46" s="29" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="14"/>
+      <c r="A47" s="33"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="30"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="14"/>
+      <c r="A48" s="33"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="30"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="14"/>
+      <c r="A49" s="33"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="30"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="14"/>
+      <c r="A50" s="33"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="30"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="14"/>
+      <c r="A51" s="33"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="39"/>
+      <c r="F51" s="30"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="18"/>
-      <c r="B52" s="15"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="15"/>
+      <c r="A52" s="34"/>
+      <c r="B52" s="31"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="31"/>
     </row>
     <row r="53" spans="1:6" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="16" t="s">
+      <c r="A53" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="B53" s="13">
+      <c r="B53" s="29">
         <v>858</v>
       </c>
-      <c r="C53" s="22">
+      <c r="C53" s="35">
         <v>123552</v>
       </c>
-      <c r="D53" s="19">
+      <c r="D53" s="38">
         <v>4.7538999999999998E-2</v>
       </c>
-      <c r="E53" s="19">
+      <c r="E53" s="38">
         <v>7.6200000000000004E-2</v>
       </c>
-      <c r="F53" s="13" t="s">
+      <c r="F53" s="29" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="14"/>
+      <c r="A54" s="33"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="30"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="23"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="14"/>
+      <c r="A55" s="33"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="30"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="17"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="14"/>
+      <c r="A56" s="33"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="30"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="17"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="23"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="14"/>
+      <c r="A57" s="33"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="30"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="17"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="23"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="14"/>
+      <c r="A58" s="33"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="30"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="18"/>
-      <c r="B59" s="15"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="21"/>
-      <c r="E59" s="21"/>
-      <c r="F59" s="15"/>
+      <c r="A59" s="34"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="40"/>
+      <c r="F59" s="31"/>
     </row>
     <row r="60" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B60" s="22">
+      <c r="B60" s="35">
         <v>2860</v>
       </c>
-      <c r="C60" s="22">
+      <c r="C60" s="35">
         <v>1098240</v>
       </c>
-      <c r="D60" s="19">
+      <c r="D60" s="38">
         <v>0.42256899999999997</v>
       </c>
-      <c r="E60" s="19">
+      <c r="E60" s="38">
         <v>0.499</v>
       </c>
-      <c r="F60" s="13" t="s">
+      <c r="F60" s="29" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="17"/>
-      <c r="B61" s="23"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="14"/>
+      <c r="A61" s="33"/>
+      <c r="B61" s="36"/>
+      <c r="C61" s="36"/>
+      <c r="D61" s="39"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="30"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="17"/>
-      <c r="B62" s="23"/>
-      <c r="C62" s="23"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="14"/>
+      <c r="A62" s="33"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="39"/>
+      <c r="E62" s="39"/>
+      <c r="F62" s="30"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="17"/>
-      <c r="B63" s="23"/>
-      <c r="C63" s="23"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="14"/>
+      <c r="A63" s="33"/>
+      <c r="B63" s="36"/>
+      <c r="C63" s="36"/>
+      <c r="D63" s="39"/>
+      <c r="E63" s="39"/>
+      <c r="F63" s="30"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="17"/>
-      <c r="B64" s="23"/>
-      <c r="C64" s="23"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="14"/>
+      <c r="A64" s="33"/>
+      <c r="B64" s="36"/>
+      <c r="C64" s="36"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="30"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="17"/>
-      <c r="B65" s="23"/>
-      <c r="C65" s="23"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="14"/>
+      <c r="A65" s="33"/>
+      <c r="B65" s="36"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="39"/>
+      <c r="E65" s="39"/>
+      <c r="F65" s="30"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="18"/>
-      <c r="B66" s="24"/>
-      <c r="C66" s="24"/>
-      <c r="D66" s="21"/>
-      <c r="E66" s="21"/>
-      <c r="F66" s="15"/>
+      <c r="A66" s="34"/>
+      <c r="B66" s="37"/>
+      <c r="C66" s="37"/>
+      <c r="D66" s="40"/>
+      <c r="E66" s="40"/>
+      <c r="F66" s="31"/>
     </row>
     <row r="67" spans="1:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="16" t="s">
+      <c r="A67" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="B67" s="22">
+      <c r="B67" s="35">
         <v>1277</v>
       </c>
-      <c r="C67" s="22">
+      <c r="C67" s="35">
         <v>1302540</v>
       </c>
-      <c r="D67" s="19">
+      <c r="D67" s="38">
         <v>0.50117699999999998</v>
       </c>
-      <c r="E67" s="25">
+      <c r="E67" s="41">
         <v>1</v>
       </c>
-      <c r="F67" s="13" t="s">
+      <c r="F67" s="29" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="17"/>
-      <c r="B68" s="23"/>
-      <c r="C68" s="23"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="26"/>
-      <c r="F68" s="14"/>
+      <c r="A68" s="33"/>
+      <c r="B68" s="36"/>
+      <c r="C68" s="36"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="42"/>
+      <c r="F68" s="30"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="17"/>
-      <c r="B69" s="23"/>
-      <c r="C69" s="23"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="26"/>
-      <c r="F69" s="14"/>
+      <c r="A69" s="33"/>
+      <c r="B69" s="36"/>
+      <c r="C69" s="36"/>
+      <c r="D69" s="39"/>
+      <c r="E69" s="42"/>
+      <c r="F69" s="30"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="17"/>
-      <c r="B70" s="23"/>
-      <c r="C70" s="23"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="26"/>
-      <c r="F70" s="14"/>
+      <c r="A70" s="33"/>
+      <c r="B70" s="36"/>
+      <c r="C70" s="36"/>
+      <c r="D70" s="39"/>
+      <c r="E70" s="42"/>
+      <c r="F70" s="30"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="17"/>
-      <c r="B71" s="23"/>
-      <c r="C71" s="23"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="26"/>
-      <c r="F71" s="14"/>
+      <c r="A71" s="33"/>
+      <c r="B71" s="36"/>
+      <c r="C71" s="36"/>
+      <c r="D71" s="39"/>
+      <c r="E71" s="42"/>
+      <c r="F71" s="30"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="17"/>
-      <c r="B72" s="23"/>
-      <c r="C72" s="23"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="26"/>
-      <c r="F72" s="14"/>
+      <c r="A72" s="33"/>
+      <c r="B72" s="36"/>
+      <c r="C72" s="36"/>
+      <c r="D72" s="39"/>
+      <c r="E72" s="42"/>
+      <c r="F72" s="30"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="18"/>
-      <c r="B73" s="24"/>
-      <c r="C73" s="24"/>
-      <c r="D73" s="21"/>
-      <c r="E73" s="27"/>
-      <c r="F73" s="15"/>
+      <c r="A73" s="34"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="37"/>
+      <c r="D73" s="40"/>
+      <c r="E73" s="43"/>
+      <c r="F73" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="F11:F17"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="C4:C10"/>
+    <mergeCell ref="D4:D10"/>
+    <mergeCell ref="E4:E10"/>
+    <mergeCell ref="F4:F10"/>
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="C11:C17"/>
+    <mergeCell ref="D11:D17"/>
+    <mergeCell ref="E11:E17"/>
+    <mergeCell ref="F25:F31"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="C18:C24"/>
+    <mergeCell ref="D18:D24"/>
+    <mergeCell ref="E18:E24"/>
+    <mergeCell ref="F18:F24"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="C25:C31"/>
+    <mergeCell ref="D25:D31"/>
+    <mergeCell ref="E25:E31"/>
+    <mergeCell ref="F39:F45"/>
+    <mergeCell ref="A32:A38"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="D32:D38"/>
+    <mergeCell ref="E32:E38"/>
+    <mergeCell ref="F32:F38"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="B39:B45"/>
+    <mergeCell ref="C39:C45"/>
+    <mergeCell ref="D39:D45"/>
+    <mergeCell ref="E39:E45"/>
+    <mergeCell ref="F53:F59"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="C46:C52"/>
+    <mergeCell ref="D46:D52"/>
+    <mergeCell ref="E46:E52"/>
+    <mergeCell ref="F46:F52"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="B53:B59"/>
+    <mergeCell ref="C53:C59"/>
+    <mergeCell ref="D53:D59"/>
+    <mergeCell ref="E53:E59"/>
     <mergeCell ref="F67:F73"/>
     <mergeCell ref="A60:A66"/>
     <mergeCell ref="B60:B66"/>
@@ -6231,54 +6279,6 @@
     <mergeCell ref="C67:C73"/>
     <mergeCell ref="D67:D73"/>
     <mergeCell ref="E67:E73"/>
-    <mergeCell ref="F53:F59"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="C46:C52"/>
-    <mergeCell ref="D46:D52"/>
-    <mergeCell ref="E46:E52"/>
-    <mergeCell ref="F46:F52"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="B53:B59"/>
-    <mergeCell ref="C53:C59"/>
-    <mergeCell ref="D53:D59"/>
-    <mergeCell ref="E53:E59"/>
-    <mergeCell ref="F39:F45"/>
-    <mergeCell ref="A32:A38"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="D32:D38"/>
-    <mergeCell ref="E32:E38"/>
-    <mergeCell ref="F32:F38"/>
-    <mergeCell ref="A39:A45"/>
-    <mergeCell ref="B39:B45"/>
-    <mergeCell ref="C39:C45"/>
-    <mergeCell ref="D39:D45"/>
-    <mergeCell ref="E39:E45"/>
-    <mergeCell ref="F25:F31"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="C18:C24"/>
-    <mergeCell ref="D18:D24"/>
-    <mergeCell ref="E18:E24"/>
-    <mergeCell ref="F18:F24"/>
-    <mergeCell ref="A25:A31"/>
-    <mergeCell ref="B25:B31"/>
-    <mergeCell ref="C25:C31"/>
-    <mergeCell ref="D25:D31"/>
-    <mergeCell ref="E25:E31"/>
-    <mergeCell ref="F11:F17"/>
-    <mergeCell ref="A4:A10"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="C4:C10"/>
-    <mergeCell ref="D4:D10"/>
-    <mergeCell ref="E4:E10"/>
-    <mergeCell ref="F4:F10"/>
-    <mergeCell ref="A11:A17"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="C11:C17"/>
-    <mergeCell ref="D11:D17"/>
-    <mergeCell ref="E11:E17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" location="Straight_flush" tooltip="Hand rankings" display="https://en.wikipedia.org/wiki/Hand_rankings - Straight_flush"/>

</xml_diff>

<commit_message>
Adding support for Protractor, creating a few tests and modifying html for better element selectors.
</commit_message>
<xml_diff>
--- a/docs/Project Details.xlsx
+++ b/docs/Project Details.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="17970" windowHeight="24915"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="17970" windowHeight="24915"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
@@ -27,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="139">
   <si>
     <t>Investigate ECMAScript instead of Lodash</t>
   </si>
   <si>
-    <t>Create integration testing</t>
-  </si>
-  <si>
     <t>Create poker hand ranking system</t>
   </si>
   <si>
@@ -47,9 +44,6 @@
     <t>Add calls to Amazon Lambda</t>
   </si>
   <si>
-    <t>Add calls to Google Functions</t>
-  </si>
-  <si>
     <t>Add calls to Azure Functions</t>
   </si>
   <si>
@@ -104,9 +98,6 @@
     <t>Medium</t>
   </si>
   <si>
-    <t>Create probabilty ranking system</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
@@ -197,9 +188,6 @@
     <t>Sort: Rank, greatest first, first result</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -317,9 +305,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Refactor card, hand, dealer, etc.</t>
   </si>
   <si>
@@ -329,18 +314,9 @@
     <t>Add poker card pictures</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>Create poker hand visualization</t>
   </si>
   <si>
-    <t>Create unit tests  for hand, card, dealer, etc.</t>
-  </si>
-  <si>
-    <t>Create unit tests  for sorter, evaluator, etc.</t>
-  </si>
-  <si>
     <t>isSequence</t>
   </si>
   <si>
@@ -447,6 +423,27 @@
   </si>
   <si>
     <t>}]</t>
+  </si>
+  <si>
+    <t>Create tests  for hand, card, dealer, etc.</t>
+  </si>
+  <si>
+    <t>Create  tests for sorter, evaluator, etc.</t>
+  </si>
+  <si>
+    <t>Create end to end testing</t>
+  </si>
+  <si>
+    <t>Install protractor, webdriver</t>
+  </si>
+  <si>
+    <t>Sequencer: byRank, HighCard: Ace</t>
+  </si>
+  <si>
+    <t>Sequencer: byRank</t>
+  </si>
+  <si>
+    <t>Add calls to Google Cloud Functions</t>
   </si>
 </sst>
 </file>
@@ -753,6 +750,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -760,15 +766,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4339,7 +4336,7 @@
   <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4349,348 +4346,348 @@
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>102</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>96</v>
+        <v>132</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>100</v>
+        <v>2</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" t="s">
-        <v>98</v>
-      </c>
-      <c r="C31" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C45" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>138</v>
       </c>
       <c r="C46" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B66" t="s">
         <v>0</v>
@@ -4718,109 +4715,109 @@
     <row r="2" spans="1:11" s="21" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
       <c r="B2" s="21" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C2" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>31</v>
-      </c>
       <c r="F2" s="21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G2" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="K2" s="21" t="s">
         <v>40</v>
-      </c>
-      <c r="I2" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="K2" s="21" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B5" s="15">
         <v>0</v>
@@ -4855,7 +4852,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B6" s="15">
         <v>0</v>
@@ -4890,7 +4887,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B7" s="15">
         <v>0</v>
@@ -4925,14 +4922,14 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B8" s="24" t="str">
         <f>TEXT("==Ace","")</f>
         <v>==Ace</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -4945,170 +4942,170 @@
     </row>
     <row r="9" spans="1:11" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="27"/>
       <c r="D9" s="27" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="27" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H9" s="27"/>
       <c r="I9" s="27"/>
       <c r="J9" s="28" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="K9" s="27"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -5122,7 +5119,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5135,7 +5132,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -5143,30 +5140,30 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -5174,30 +5171,30 @@
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -5205,30 +5202,30 @@
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -5236,41 +5233,41 @@
         <v>4</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -5278,30 +5275,30 @@
         <v>5</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C20" s="6"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -5309,30 +5306,30 @@
         <v>6</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C24" s="6"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E25" t="s">
-        <v>56</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -5340,30 +5337,30 @@
         <v>7</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C28" s="6"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E29" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C30" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E30" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -5371,41 +5368,41 @@
         <v>8</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C32" s="6"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C33" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E33" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C34" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E34" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C35" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E35" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -5413,30 +5410,30 @@
         <v>9</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C37" s="6"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C38" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D38" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E38" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C39" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E39" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -5444,41 +5441,41 @@
         <v>10</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C41" s="6"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C42" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D42" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E42" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C43" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D43" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E43" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C44" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D44" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -5494,7 +5491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11:D17"/>
     </sheetView>
   </sheetViews>
@@ -5509,37 +5506,37 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B4" s="29">
         <v>1</v>
@@ -5547,67 +5544,67 @@
       <c r="C4" s="29">
         <v>4</v>
       </c>
-      <c r="D4" s="38">
+      <c r="D4" s="35">
         <v>1.5400000000000001E-6</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="35">
         <v>1.5400000000000001E-6</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="33"/>
       <c r="B5" s="30"/>
       <c r="C5" s="30"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="33"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
       <c r="F6" s="30"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="33"/>
       <c r="B7" s="30"/>
       <c r="C7" s="30"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
       <c r="F7" s="30"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="33"/>
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
       <c r="F8" s="30"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
       <c r="B9" s="30"/>
       <c r="C9" s="30"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
       <c r="F9" s="30"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="34"/>
       <c r="B10" s="31"/>
       <c r="C10" s="31"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
       <c r="F10" s="31"/>
     </row>
     <row r="11" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B11" s="29">
         <v>9</v>
@@ -5615,67 +5612,67 @@
       <c r="C11" s="29">
         <v>36</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="35">
         <v>1.3900000000000001E-5</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="35">
         <v>1.5E-5</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="33"/>
       <c r="B12" s="30"/>
       <c r="C12" s="30"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
       <c r="F12" s="30"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="33"/>
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
       <c r="F13" s="30"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="33"/>
       <c r="B14" s="30"/>
       <c r="C14" s="30"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
       <c r="F14" s="30"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
       <c r="B15" s="30"/>
       <c r="C15" s="30"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
       <c r="F15" s="30"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
       <c r="B16" s="30"/>
       <c r="C16" s="30"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
       <c r="F16" s="30"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="34"/>
       <c r="B17" s="31"/>
       <c r="C17" s="31"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
       <c r="F17" s="31"/>
     </row>
     <row r="18" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B18" s="29">
         <v>156</v>
@@ -5683,542 +5680,590 @@
       <c r="C18" s="29">
         <v>624</v>
       </c>
-      <c r="D18" s="38">
+      <c r="D18" s="35">
         <v>2.4000000000000001E-4</v>
       </c>
-      <c r="E18" s="38">
+      <c r="E18" s="35">
         <v>2.5599999999999999E-4</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="33"/>
       <c r="B19" s="30"/>
       <c r="C19" s="30"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
       <c r="F19" s="30"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="33"/>
       <c r="B20" s="30"/>
       <c r="C20" s="30"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
       <c r="F20" s="30"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="33"/>
       <c r="B21" s="30"/>
       <c r="C21" s="30"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
       <c r="F21" s="30"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="33"/>
       <c r="B22" s="30"/>
       <c r="C22" s="30"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
       <c r="F22" s="30"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="33"/>
       <c r="B23" s="30"/>
       <c r="C23" s="30"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
       <c r="F23" s="30"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="34"/>
       <c r="B24" s="31"/>
       <c r="C24" s="31"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
       <c r="F24" s="31"/>
     </row>
     <row r="25" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B25" s="29">
         <v>156</v>
       </c>
-      <c r="C25" s="35">
+      <c r="C25" s="38">
         <v>3744</v>
       </c>
-      <c r="D25" s="38">
+      <c r="D25" s="35">
         <v>1.441E-3</v>
       </c>
-      <c r="E25" s="38">
+      <c r="E25" s="35">
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="F25" s="29" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="33"/>
       <c r="B26" s="30"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
       <c r="F26" s="30"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="33"/>
       <c r="B27" s="30"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
       <c r="F27" s="30"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="33"/>
       <c r="B28" s="30"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
       <c r="F28" s="30"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="33"/>
       <c r="B29" s="30"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
       <c r="F29" s="30"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="33"/>
       <c r="B30" s="30"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
       <c r="F30" s="30"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="34"/>
       <c r="B31" s="31"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
       <c r="F31" s="31"/>
     </row>
     <row r="32" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="B32" s="35">
+        <v>72</v>
+      </c>
+      <c r="B32" s="38">
         <v>1277</v>
       </c>
-      <c r="C32" s="35">
+      <c r="C32" s="38">
         <v>5108</v>
       </c>
-      <c r="D32" s="38">
+      <c r="D32" s="35">
         <v>1.9650000000000002E-3</v>
       </c>
-      <c r="E32" s="38">
+      <c r="E32" s="35">
         <v>3.6700000000000001E-3</v>
       </c>
       <c r="F32" s="29" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="33"/>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
       <c r="F33" s="30"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="33"/>
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
       <c r="F34" s="30"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="33"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
       <c r="F35" s="30"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="33"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
       <c r="F36" s="30"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="33"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
       <c r="F37" s="30"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="34"/>
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="40"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
       <c r="F38" s="31"/>
     </row>
     <row r="39" spans="1:6" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="32" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B39" s="29">
         <v>10</v>
       </c>
-      <c r="C39" s="35">
+      <c r="C39" s="38">
         <v>10200</v>
       </c>
-      <c r="D39" s="38">
+      <c r="D39" s="35">
         <v>3.9249999999999997E-3</v>
       </c>
-      <c r="E39" s="38">
+      <c r="E39" s="35">
         <v>7.6E-3</v>
       </c>
       <c r="F39" s="29" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="33"/>
       <c r="B40" s="30"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="39"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
       <c r="F40" s="30"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="33"/>
       <c r="B41" s="30"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="36"/>
       <c r="F41" s="30"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="33"/>
       <c r="B42" s="30"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
       <c r="F42" s="30"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="33"/>
       <c r="B43" s="30"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
       <c r="F43" s="30"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="33"/>
       <c r="B44" s="30"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
       <c r="F44" s="30"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="34"/>
       <c r="B45" s="31"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="40"/>
-      <c r="E45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
       <c r="F45" s="31"/>
     </row>
     <row r="46" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B46" s="29">
         <v>858</v>
       </c>
-      <c r="C46" s="35">
+      <c r="C46" s="38">
         <v>54912</v>
       </c>
-      <c r="D46" s="38">
+      <c r="D46" s="35">
         <v>2.1128000000000001E-2</v>
       </c>
-      <c r="E46" s="38">
+      <c r="E46" s="35">
         <v>2.87E-2</v>
       </c>
       <c r="F46" s="29" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="33"/>
       <c r="B47" s="30"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
       <c r="F47" s="30"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="33"/>
       <c r="B48" s="30"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
+      <c r="C48" s="39"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="36"/>
       <c r="F48" s="30"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="33"/>
       <c r="B49" s="30"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="39"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="36"/>
       <c r="F49" s="30"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="33"/>
       <c r="B50" s="30"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="39"/>
-      <c r="E50" s="39"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="36"/>
       <c r="F50" s="30"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="33"/>
       <c r="B51" s="30"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="39"/>
-      <c r="E51" s="39"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="36"/>
+      <c r="E51" s="36"/>
       <c r="F51" s="30"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="34"/>
       <c r="B52" s="31"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="40"/>
-      <c r="E52" s="40"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="37"/>
       <c r="F52" s="31"/>
     </row>
     <row r="53" spans="1:6" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="32" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B53" s="29">
         <v>858</v>
       </c>
-      <c r="C53" s="35">
+      <c r="C53" s="38">
         <v>123552</v>
       </c>
-      <c r="D53" s="38">
+      <c r="D53" s="35">
         <v>4.7538999999999998E-2</v>
       </c>
-      <c r="E53" s="38">
+      <c r="E53" s="35">
         <v>7.6200000000000004E-2</v>
       </c>
       <c r="F53" s="29" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="33"/>
       <c r="B54" s="30"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="39"/>
+      <c r="C54" s="39"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="36"/>
       <c r="F54" s="30"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="33"/>
       <c r="B55" s="30"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
       <c r="F55" s="30"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="33"/>
       <c r="B56" s="30"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="39"/>
-      <c r="E56" s="39"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="36"/>
       <c r="F56" s="30"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="33"/>
       <c r="B57" s="30"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="39"/>
-      <c r="E57" s="39"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="36"/>
       <c r="F57" s="30"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="33"/>
       <c r="B58" s="30"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="39"/>
-      <c r="E58" s="39"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="36"/>
+      <c r="E58" s="36"/>
       <c r="F58" s="30"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="34"/>
       <c r="B59" s="31"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="40"/>
-      <c r="E59" s="40"/>
+      <c r="C59" s="40"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
       <c r="F59" s="31"/>
     </row>
     <row r="60" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B60" s="35">
+        <v>80</v>
+      </c>
+      <c r="B60" s="38">
         <v>2860</v>
       </c>
-      <c r="C60" s="35">
+      <c r="C60" s="38">
         <v>1098240</v>
       </c>
-      <c r="D60" s="38">
+      <c r="D60" s="35">
         <v>0.42256899999999997</v>
       </c>
-      <c r="E60" s="38">
+      <c r="E60" s="35">
         <v>0.499</v>
       </c>
       <c r="F60" s="29" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="33"/>
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="39"/>
+      <c r="B61" s="39"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="36"/>
+      <c r="E61" s="36"/>
       <c r="F61" s="30"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="33"/>
-      <c r="B62" s="36"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="39"/>
-      <c r="E62" s="39"/>
+      <c r="B62" s="39"/>
+      <c r="C62" s="39"/>
+      <c r="D62" s="36"/>
+      <c r="E62" s="36"/>
       <c r="F62" s="30"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="33"/>
-      <c r="B63" s="36"/>
-      <c r="C63" s="36"/>
-      <c r="D63" s="39"/>
-      <c r="E63" s="39"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="39"/>
+      <c r="D63" s="36"/>
+      <c r="E63" s="36"/>
       <c r="F63" s="30"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="33"/>
-      <c r="B64" s="36"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="39"/>
-      <c r="E64" s="39"/>
+      <c r="B64" s="39"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="36"/>
+      <c r="E64" s="36"/>
       <c r="F64" s="30"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="33"/>
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="39"/>
-      <c r="E65" s="39"/>
+      <c r="B65" s="39"/>
+      <c r="C65" s="39"/>
+      <c r="D65" s="36"/>
+      <c r="E65" s="36"/>
       <c r="F65" s="30"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="34"/>
-      <c r="B66" s="37"/>
-      <c r="C66" s="37"/>
-      <c r="D66" s="40"/>
-      <c r="E66" s="40"/>
+      <c r="B66" s="40"/>
+      <c r="C66" s="40"/>
+      <c r="D66" s="37"/>
+      <c r="E66" s="37"/>
       <c r="F66" s="31"/>
     </row>
     <row r="67" spans="1:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="B67" s="35">
+        <v>82</v>
+      </c>
+      <c r="B67" s="38">
         <v>1277</v>
       </c>
-      <c r="C67" s="35">
+      <c r="C67" s="38">
         <v>1302540</v>
       </c>
-      <c r="D67" s="38">
+      <c r="D67" s="35">
         <v>0.50117699999999998</v>
       </c>
       <c r="E67" s="41">
         <v>1</v>
       </c>
       <c r="F67" s="29" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="33"/>
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="39"/>
+      <c r="B68" s="39"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="36"/>
       <c r="E68" s="42"/>
       <c r="F68" s="30"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="33"/>
-      <c r="B69" s="36"/>
-      <c r="C69" s="36"/>
-      <c r="D69" s="39"/>
+      <c r="B69" s="39"/>
+      <c r="C69" s="39"/>
+      <c r="D69" s="36"/>
       <c r="E69" s="42"/>
       <c r="F69" s="30"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="33"/>
-      <c r="B70" s="36"/>
-      <c r="C70" s="36"/>
-      <c r="D70" s="39"/>
+      <c r="B70" s="39"/>
+      <c r="C70" s="39"/>
+      <c r="D70" s="36"/>
       <c r="E70" s="42"/>
       <c r="F70" s="30"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="33"/>
-      <c r="B71" s="36"/>
-      <c r="C71" s="36"/>
-      <c r="D71" s="39"/>
+      <c r="B71" s="39"/>
+      <c r="C71" s="39"/>
+      <c r="D71" s="36"/>
       <c r="E71" s="42"/>
       <c r="F71" s="30"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="33"/>
-      <c r="B72" s="36"/>
-      <c r="C72" s="36"/>
-      <c r="D72" s="39"/>
+      <c r="B72" s="39"/>
+      <c r="C72" s="39"/>
+      <c r="D72" s="36"/>
       <c r="E72" s="42"/>
       <c r="F72" s="30"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="34"/>
-      <c r="B73" s="37"/>
-      <c r="C73" s="37"/>
-      <c r="D73" s="40"/>
+      <c r="B73" s="40"/>
+      <c r="C73" s="40"/>
+      <c r="D73" s="37"/>
       <c r="E73" s="43"/>
       <c r="F73" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="F67:F73"/>
+    <mergeCell ref="A60:A66"/>
+    <mergeCell ref="B60:B66"/>
+    <mergeCell ref="C60:C66"/>
+    <mergeCell ref="D60:D66"/>
+    <mergeCell ref="E60:E66"/>
+    <mergeCell ref="F60:F66"/>
+    <mergeCell ref="A67:A73"/>
+    <mergeCell ref="B67:B73"/>
+    <mergeCell ref="C67:C73"/>
+    <mergeCell ref="D67:D73"/>
+    <mergeCell ref="E67:E73"/>
+    <mergeCell ref="F53:F59"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="C46:C52"/>
+    <mergeCell ref="D46:D52"/>
+    <mergeCell ref="E46:E52"/>
+    <mergeCell ref="F46:F52"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="B53:B59"/>
+    <mergeCell ref="C53:C59"/>
+    <mergeCell ref="D53:D59"/>
+    <mergeCell ref="E53:E59"/>
+    <mergeCell ref="F39:F45"/>
+    <mergeCell ref="A32:A38"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="D32:D38"/>
+    <mergeCell ref="E32:E38"/>
+    <mergeCell ref="F32:F38"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="B39:B45"/>
+    <mergeCell ref="C39:C45"/>
+    <mergeCell ref="D39:D45"/>
+    <mergeCell ref="E39:E45"/>
+    <mergeCell ref="F25:F31"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="C18:C24"/>
+    <mergeCell ref="D18:D24"/>
+    <mergeCell ref="E18:E24"/>
+    <mergeCell ref="F18:F24"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="C25:C31"/>
+    <mergeCell ref="D25:D31"/>
+    <mergeCell ref="E25:E31"/>
     <mergeCell ref="F11:F17"/>
     <mergeCell ref="A4:A10"/>
     <mergeCell ref="B4:B10"/>
@@ -6231,54 +6276,6 @@
     <mergeCell ref="C11:C17"/>
     <mergeCell ref="D11:D17"/>
     <mergeCell ref="E11:E17"/>
-    <mergeCell ref="F25:F31"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="C18:C24"/>
-    <mergeCell ref="D18:D24"/>
-    <mergeCell ref="E18:E24"/>
-    <mergeCell ref="F18:F24"/>
-    <mergeCell ref="A25:A31"/>
-    <mergeCell ref="B25:B31"/>
-    <mergeCell ref="C25:C31"/>
-    <mergeCell ref="D25:D31"/>
-    <mergeCell ref="E25:E31"/>
-    <mergeCell ref="F39:F45"/>
-    <mergeCell ref="A32:A38"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="D32:D38"/>
-    <mergeCell ref="E32:E38"/>
-    <mergeCell ref="F32:F38"/>
-    <mergeCell ref="A39:A45"/>
-    <mergeCell ref="B39:B45"/>
-    <mergeCell ref="C39:C45"/>
-    <mergeCell ref="D39:D45"/>
-    <mergeCell ref="E39:E45"/>
-    <mergeCell ref="F53:F59"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="C46:C52"/>
-    <mergeCell ref="D46:D52"/>
-    <mergeCell ref="E46:E52"/>
-    <mergeCell ref="F46:F52"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="B53:B59"/>
-    <mergeCell ref="C53:C59"/>
-    <mergeCell ref="D53:D59"/>
-    <mergeCell ref="E53:E59"/>
-    <mergeCell ref="F67:F73"/>
-    <mergeCell ref="A60:A66"/>
-    <mergeCell ref="B60:B66"/>
-    <mergeCell ref="C60:C66"/>
-    <mergeCell ref="D60:D66"/>
-    <mergeCell ref="E60:E66"/>
-    <mergeCell ref="F60:F66"/>
-    <mergeCell ref="A67:A73"/>
-    <mergeCell ref="B67:B73"/>
-    <mergeCell ref="C67:C73"/>
-    <mergeCell ref="D67:D73"/>
-    <mergeCell ref="E67:E73"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" location="Straight_flush" tooltip="Hand rankings" display="https://en.wikipedia.org/wiki/Hand_rankings - Straight_flush"/>

</xml_diff>